<commit_message>
start prefix wrangle, add data progress function
</commit_message>
<xml_diff>
--- a/input/地词合并表单.xlsx
+++ b/input/地词合并表单.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad\Desktop\TJlab\Tang\chinese_poetry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TJlab\Tang\chinese_poetry\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C225A65-021D-4808-B523-5A3DDC6872BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D06272-BE77-4A91-BFC5-DF8D5C89A0B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CEB0267F-DDE7-4FC5-98D2-7BBADDA4D0E5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>终南山</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -350,6 +350,18 @@
   </si>
   <si>
     <t>渭川道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>素浐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长安</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -746,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290E6562-4E47-4BE0-B0BB-E30B313D32B9}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -889,6 +901,9 @@
       <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -919,6 +934,9 @@
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -930,19 +948,49 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -977,152 +1025,123 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" t="s">
-        <v>91</v>
+        <v>64</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A26" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="B26" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="B27" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="A28" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish qujiang co-occur first round
</commit_message>
<xml_diff>
--- a/input/地词合并表单.xlsx
+++ b/input/地词合并表单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TJlab\Tang\chinese_poetry\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D06272-BE77-4A91-BFC5-DF8D5C89A0B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1008D74C-7903-4538-8954-8C86ADF823A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CEB0267F-DDE7-4FC5-98D2-7BBADDA4D0E5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>终南山</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -362,6 +362,117 @@
   </si>
   <si>
     <t>长安</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曲江</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曲池</t>
+  </si>
+  <si>
+    <t>乐游原</t>
+  </si>
+  <si>
+    <t>乐游园</t>
+  </si>
+  <si>
+    <t>慈恩</t>
+  </si>
+  <si>
+    <t>慈恩寺</t>
+  </si>
+  <si>
+    <t>乐游</t>
+  </si>
+  <si>
+    <t>芙蓉园</t>
+  </si>
+  <si>
+    <t>芙蓉池</t>
+  </si>
+  <si>
+    <t>芙蓉苑</t>
+  </si>
+  <si>
+    <t>曲水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>杏园</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>杏花园</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大慈恩寺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曲沼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>皇畿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>皇州</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杏苑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>宜春苑</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>下苑</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曲岸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曲地</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -369,7 +480,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +518,12 @@
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
@@ -758,15 +875,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290E6562-4E47-4BE0-B0BB-E30B313D32B9}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -780,7 +897,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -806,7 +923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -822,7 +939,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -836,7 +953,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -886,7 +1003,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -894,7 +1011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -905,7 +1022,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -913,7 +1030,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -924,7 +1041,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -938,7 +1055,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -946,7 +1063,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>106</v>
       </c>
@@ -992,8 +1109,14 @@
       <c r="O12" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1001,7 +1124,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -1012,7 +1135,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -1023,7 +1146,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1031,7 +1154,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -1042,7 +1165,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>63</v>
       </c>
@@ -1056,7 +1179,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>66</v>
       </c>
@@ -1064,7 +1187,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
@@ -1072,7 +1195,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -1083,7 +1206,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>75</v>
       </c>
@@ -1094,7 +1217,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>77</v>
       </c>
@@ -1102,7 +1225,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>88</v>
       </c>
@@ -1113,7 +1236,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>92</v>
       </c>
@@ -1121,7 +1244,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>95</v>
       </c>
@@ -1129,7 +1252,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>98</v>
       </c>
@@ -1137,12 +1260,84 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
qujiang co-occur second round
</commit_message>
<xml_diff>
--- a/input/地词合并表单.xlsx
+++ b/input/地词合并表单.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TJlab\Tang\chinese_poetry\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1008D74C-7903-4538-8954-8C86ADF823A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AF8B81-760A-440C-93B3-5418DFFB332C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CEB0267F-DDE7-4FC5-98D2-7BBADDA4D0E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>终南山</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -473,6 +473,10 @@
   </si>
   <si>
     <t>曲地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雁塔</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -878,7 +882,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1309,6 +1313,9 @@
       <c r="C31" t="s">
         <v>120</v>
       </c>
+      <c r="D31" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">

</xml_diff>